<commit_message>
renamed + tool added
</commit_message>
<xml_diff>
--- a/3-Checklists/📋 Design tool inventory.xlsx
+++ b/3-Checklists/📋 Design tool inventory.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="192">
   <si>
     <t>Tool</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Building clickable prototypes</t>
+  </si>
+  <si>
+    <t>Figma</t>
   </si>
   <si>
     <t>TryMyUI</t>
@@ -829,104 +832,108 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2" t="s">
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2" t="s">
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2" t="s">
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2" t="s">
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2" t="s">
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2" t="s">
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="2" t="s">
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="2" t="s">
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" s="3"/>
@@ -4859,6 +4866,10 @@
     <row r="1000">
       <c r="A1000" s="3"/>
       <c r="B1000" s="3"/>
+    </row>
+    <row r="1001">
+      <c r="A1001" s="3"/>
+      <c r="B1001" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId2"/>
@@ -4906,98 +4917,98 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16">
@@ -8961,18 +8972,18 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
@@ -8980,79 +8991,79 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14">
@@ -13031,7 +13042,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2">
@@ -13054,124 +13065,124 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="C14" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" s="3"/>
     </row>
@@ -18099,98 +18110,98 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14">
@@ -22174,74 +22185,74 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11">
@@ -22249,15 +22260,15 @@
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13">
@@ -22265,23 +22276,23 @@
         <v>4</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19">
@@ -26240,10 +26251,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2">
@@ -26251,7 +26262,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>5</v>
@@ -26259,233 +26270,233 @@
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>119</v>
-      </c>
       <c r="C4" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="7" t="s">
-        <v>20</v>
+      <c r="C8" s="7" t="s">
+        <v>26</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>123</v>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="s">
+        <v>27</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="B9" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>123</v>
-      </c>
       <c r="C22" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -26519,177 +26530,177 @@
         <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D2" s="13"/>
     </row>
     <row r="3">
       <c r="B3" s="14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D3" s="15"/>
     </row>
     <row r="4">
       <c r="B4" s="14" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D4" s="15"/>
     </row>
     <row r="5">
       <c r="B5" s="15" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D5" s="15"/>
     </row>
     <row r="6">
       <c r="B6" s="15" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D6" s="15"/>
     </row>
     <row r="7">
       <c r="B7" s="15" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D7" s="15"/>
     </row>
     <row r="8">
       <c r="B8" s="15" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C8" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="D8" s="15"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="D8" s="15"/>
-    </row>
-    <row r="9">
-      <c r="B9" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>166</v>
-      </c>
       <c r="D10" s="15" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="14" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D12" s="5"/>
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="15" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="14" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D15" s="5"/>
     </row>
     <row r="16">
       <c r="B16" s="15" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="14" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="15" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D18" s="5"/>
     </row>

</xml_diff>